<commit_message>
Update parameters and reconstruction file
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\wiki\Praca_licencjacka\licencjat\Three-dimentional-tumor-reconstruction\Three-dimensional-tumor-reconstruction-algorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wikto\Documents\Python25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DE23EC9-9B86-476B-8A4D-310F54773E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD7CDBC0-0BF0-466C-9E62-656303D5C9E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="3" xr2:uid="{06D7DBA6-62A4-477F-BDDB-CC1BD74D9D43}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" firstSheet="1" activeTab="4" xr2:uid="{06D7DBA6-62A4-477F-BDDB-CC1BD74D9D43}"/>
   </bookViews>
   <sheets>
     <sheet name="1338" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="15">
   <si>
     <t>Data</t>
   </si>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -155,7 +155,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -703,24 +702,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBFFC31-F43E-4A7A-AAAA-350359871149}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.3828125" customWidth="1"/>
     <col min="2" max="2" width="13.61328125" customWidth="1"/>
-    <col min="3" max="3" width="18.15234375" customWidth="1"/>
-    <col min="4" max="4" width="16.4609375" customWidth="1"/>
-    <col min="5" max="5" width="16.53515625" customWidth="1"/>
-    <col min="6" max="6" width="18.61328125" customWidth="1"/>
-    <col min="7" max="7" width="15.69140625" customWidth="1"/>
+    <col min="3" max="3" width="16.4609375" customWidth="1"/>
+    <col min="4" max="4" width="16.53515625" customWidth="1"/>
+    <col min="5" max="5" width="18.61328125" customWidth="1"/>
+    <col min="6" max="6" width="15.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -728,22 +726,19 @@
         <v>14</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>45355</v>
       </c>
@@ -751,22 +746,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>63.597000000000001</v>
+        <v>57.31</v>
       </c>
       <c r="D2">
-        <v>57.31</v>
+        <v>0.1016</v>
       </c>
       <c r="E2">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F2">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G2">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>45355</v>
       </c>
@@ -774,22 +766,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>84.153999999999996</v>
+        <v>76.41</v>
       </c>
       <c r="D3">
-        <v>76.41</v>
+        <v>0.1016</v>
       </c>
       <c r="E3">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F3">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G3">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>45359</v>
       </c>
@@ -797,22 +786,19 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>88.29</v>
+        <v>75.75</v>
       </c>
       <c r="D4">
-        <v>75.75</v>
+        <v>0.1016</v>
       </c>
       <c r="E4">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F4">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G4">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>45359</v>
       </c>
@@ -820,22 +806,19 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>96.745000000000005</v>
+        <v>79.98</v>
       </c>
       <c r="D5">
-        <v>79.98</v>
+        <v>0.1016</v>
       </c>
       <c r="E5">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F5">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G5">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>45367</v>
       </c>
@@ -843,45 +826,39 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>321.23399999999998</v>
+        <v>265.79000000000002</v>
       </c>
       <c r="D6">
-        <v>265.79000000000002</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="E6">
-        <v>0.20319999999999999</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F6">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G6">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>45370</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>215.102</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="C7" s="6">
         <v>161.35</v>
       </c>
+      <c r="D7">
+        <v>0.1016</v>
+      </c>
       <c r="E7">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F7">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G7">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>45370</v>
       </c>
@@ -889,18 +866,15 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>310.916</v>
+        <v>225.33</v>
       </c>
       <c r="D8">
-        <v>225.33</v>
+        <v>0.1016</v>
       </c>
       <c r="E8">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F8">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G8">
         <v>14.0524999238551</v>
       </c>
     </row>
@@ -911,24 +885,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819812E4-D79A-4360-8E1B-364CA407B93A}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.84375" customWidth="1"/>
     <col min="2" max="2" width="12.61328125" customWidth="1"/>
-    <col min="3" max="3" width="20.15234375" customWidth="1"/>
-    <col min="4" max="4" width="16.15234375" customWidth="1"/>
-    <col min="5" max="5" width="15.921875" customWidth="1"/>
-    <col min="6" max="6" width="18.921875" customWidth="1"/>
-    <col min="7" max="7" width="17.07421875" customWidth="1"/>
+    <col min="3" max="3" width="16.15234375" customWidth="1"/>
+    <col min="4" max="4" width="15.921875" customWidth="1"/>
+    <col min="5" max="5" width="18.921875" customWidth="1"/>
+    <col min="6" max="6" width="17.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -936,22 +909,19 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>45355</v>
       </c>
@@ -959,22 +929,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>61.225999999999999</v>
+        <v>56.66</v>
       </c>
       <c r="D2">
-        <v>56.66</v>
+        <v>0.1016</v>
       </c>
       <c r="E2">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F2">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G2">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>45355</v>
       </c>
@@ -982,18 +949,15 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>73.974999999999994</v>
+        <v>64.61</v>
       </c>
       <c r="D3">
-        <v>64.61</v>
+        <v>0.1016</v>
       </c>
       <c r="E3">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F3">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G3">
         <v>14.0524999238551</v>
       </c>
     </row>
@@ -1004,24 +968,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97308330-8703-451E-9737-57F2A8E21B0C}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10.84375" customWidth="1"/>
     <col min="2" max="2" width="13.69140625" customWidth="1"/>
-    <col min="3" max="3" width="19.53515625" customWidth="1"/>
-    <col min="4" max="4" width="17.4609375" customWidth="1"/>
-    <col min="5" max="5" width="15.69140625" customWidth="1"/>
-    <col min="6" max="6" width="19.23046875" customWidth="1"/>
-    <col min="7" max="7" width="18.765625" customWidth="1"/>
+    <col min="3" max="3" width="17.4609375" customWidth="1"/>
+    <col min="4" max="4" width="15.69140625" customWidth="1"/>
+    <col min="5" max="5" width="19.23046875" customWidth="1"/>
+    <col min="6" max="6" width="18.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1029,22 +992,19 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>45351</v>
       </c>
@@ -1052,22 +1012,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>5.9729999999999999</v>
-      </c>
-      <c r="D2" s="6">
         <v>7.81</v>
       </c>
+      <c r="D2">
+        <v>0.1016</v>
+      </c>
       <c r="E2">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F2">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G2">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>45351</v>
       </c>
@@ -1075,22 +1032,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>9.673</v>
+        <v>17.510000000000002</v>
       </c>
       <c r="D3">
-        <v>17.510000000000002</v>
+        <v>0.1016</v>
       </c>
       <c r="E3">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F3">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G3">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>45359</v>
       </c>
@@ -1098,22 +1052,19 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>24.332000000000001</v>
+        <v>25.52</v>
       </c>
       <c r="D4">
-        <v>25.52</v>
+        <v>0.1016</v>
       </c>
       <c r="E4">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F4">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G4">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>45359</v>
       </c>
@@ -1121,22 +1072,19 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>31.617000000000001</v>
+        <v>29.19</v>
       </c>
       <c r="D5">
-        <v>29.19</v>
+        <v>0.1016</v>
       </c>
       <c r="E5">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F5">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G5">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>45370</v>
       </c>
@@ -1144,22 +1092,19 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>102.72799999999999</v>
+        <v>97.18</v>
       </c>
       <c r="D6">
-        <v>97.18</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="E6">
-        <v>0.20319999999999999</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F6">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G6">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>45355</v>
       </c>
@@ -1167,22 +1112,19 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>18.326000000000001</v>
+        <v>18.12</v>
       </c>
       <c r="D7">
-        <v>18.12</v>
+        <v>0.1016</v>
       </c>
       <c r="E7">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F7">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G7">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>45355</v>
       </c>
@@ -1190,18 +1132,15 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>21.459</v>
+        <v>23.66</v>
       </c>
       <c r="D8">
-        <v>23.66</v>
+        <v>0.1016</v>
       </c>
       <c r="E8">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F8">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G8">
         <v>14.0524999238551</v>
       </c>
     </row>
@@ -1212,24 +1151,23 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3C169FF-12D9-48EF-B71E-FD7DCE5DB5E2}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="9.921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.15234375" customWidth="1"/>
-    <col min="3" max="3" width="16.15234375" customWidth="1"/>
-    <col min="4" max="4" width="17.4609375" customWidth="1"/>
-    <col min="5" max="5" width="15.765625" customWidth="1"/>
-    <col min="6" max="6" width="19.3828125" customWidth="1"/>
-    <col min="7" max="7" width="19.4609375" customWidth="1"/>
+    <col min="3" max="3" width="17.4609375" customWidth="1"/>
+    <col min="4" max="4" width="15.765625" customWidth="1"/>
+    <col min="5" max="5" width="19.3828125" customWidth="1"/>
+    <col min="6" max="6" width="19.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1237,22 +1175,19 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>45351</v>
       </c>
@@ -1260,22 +1195,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>35.290999999999997</v>
+        <v>35.880000000000003</v>
       </c>
       <c r="D2">
-        <v>35.880000000000003</v>
+        <v>0.1016</v>
       </c>
       <c r="E2">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F2">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G2">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>45351</v>
       </c>
@@ -1283,22 +1215,19 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>37.585999999999999</v>
+        <v>36.380000000000003</v>
       </c>
       <c r="D3">
-        <v>36.380000000000003</v>
+        <v>0.1016</v>
       </c>
       <c r="E3">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F3">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G3">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>45355</v>
       </c>
@@ -1306,22 +1235,19 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>46.353999999999999</v>
+        <v>41.59</v>
       </c>
       <c r="D4">
-        <v>41.59</v>
+        <v>0.1016</v>
       </c>
       <c r="E4">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F4">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G4">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>45355</v>
       </c>
@@ -1329,22 +1255,19 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>51.304000000000002</v>
+        <v>45.9</v>
       </c>
       <c r="D5">
-        <v>45.9</v>
+        <v>0.1016</v>
       </c>
       <c r="E5">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F5">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G5">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>45359</v>
       </c>
@@ -1352,22 +1275,19 @@
         <v>7</v>
       </c>
       <c r="C6">
-        <v>67.254000000000005</v>
+        <v>58.34</v>
       </c>
       <c r="D6">
-        <v>58.34</v>
+        <v>0.20319999999999999</v>
       </c>
       <c r="E6">
-        <v>0.20319999999999999</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F6">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G6">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>45359</v>
       </c>
@@ -1375,22 +1295,19 @@
         <v>8</v>
       </c>
       <c r="C7">
-        <v>72.141999999999996</v>
+        <v>63.53</v>
       </c>
       <c r="D7">
-        <v>63.53</v>
+        <v>0.1016</v>
       </c>
       <c r="E7">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F7">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G7">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>45370</v>
       </c>
@@ -1398,22 +1315,19 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>181.929</v>
+        <v>189.55</v>
       </c>
       <c r="D8">
-        <v>189.55</v>
+        <v>0.1016</v>
       </c>
       <c r="E8">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F8">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G8">
-        <v>14.0524999238551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+        <v>14.0524999238551</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>45370</v>
       </c>
@@ -1421,18 +1335,15 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>197.74799999999999</v>
+        <v>171.08</v>
       </c>
       <c r="D9">
-        <v>171.08</v>
+        <v>0.1016</v>
       </c>
       <c r="E9">
-        <v>0.1016</v>
+        <v>13.736071586608899</v>
       </c>
       <c r="F9">
-        <v>13.736071586608899</v>
-      </c>
-      <c r="G9">
         <v>14.0524999238551</v>
       </c>
     </row>

</xml_diff>